<commit_message>
upload refined code and README.md. Removed sample datasets folder
</commit_message>
<xml_diff>
--- a/reference/data/metadata_table.xlsx
+++ b/reference/data/metadata_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEPFeatX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEPFeatX\reference\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FD3C37-2EE6-453F-9F23-FAD9AF9E6ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165C0B1A-E4A4-4C7D-B528-4FF6979BB433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -103,9 +103,6 @@
     <t>AgeGroup</t>
   </si>
   <si>
-    <t>Child</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>paired</t>
   </si>
   <si>
-    <t>rTMS</t>
-  </si>
-  <si>
-    <t>single_pulse</t>
-  </si>
-  <si>
     <t>Protocol</t>
   </si>
   <si>
@@ -163,7 +154,13 @@
     <t>Motor mapping</t>
   </si>
   <si>
-    <t>Stimulus-response</t>
+    <t>Single pulse</t>
+  </si>
+  <si>
+    <t>repetitive</t>
+  </si>
+  <si>
+    <t>RC</t>
   </si>
 </sst>
 </file>
@@ -523,19 +520,19 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -555,13 +552,13 @@
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -581,13 +578,13 @@
         <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -604,16 +601,16 @@
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -630,16 +627,16 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -656,16 +653,16 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -682,16 +679,16 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -708,16 +705,16 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -734,23 +731,22 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
       <c r="C9">
         <v>0</v>
       </c>
@@ -758,16 +754,16 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -784,16 +780,16 @@
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -810,16 +806,16 @@
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -836,16 +832,16 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>